<commit_message>
Add help files. Remove old ones
</commit_message>
<xml_diff>
--- a/tests/data/test_temlate.xlsx
+++ b/tests/data/test_temlate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://columbusglobal-my.sharepoint.com/personal/voev_columbusglobal_com/Documents/av_doc/Vehicle-Routing/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="336" documentId="8_{1C197FCC-D555-4110-9B11-7FD88CA513E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{20BD1B5E-D3CA-476C-842C-24A82962D387}"/>
+  <xr:revisionPtr revIDLastSave="339" documentId="8_{1C197FCC-D555-4110-9B11-7FD88CA513E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5F806C2E-3B7B-4882-9885-843EDF911237}"/>
   <bookViews>
-    <workbookView xWindow="1308" yWindow="1260" windowWidth="21732" windowHeight="11700" activeTab="5" xr2:uid="{A9E439BE-6E4E-4148-9B5A-691A88720DDA}"/>
+    <workbookView xWindow="12840" yWindow="288" windowWidth="21732" windowHeight="11700" activeTab="5" xr2:uid="{A9E439BE-6E4E-4148-9B5A-691A88720DDA}"/>
   </bookViews>
   <sheets>
     <sheet name="TestDescription" sheetId="7" r:id="rId1"/>
@@ -509,7 +509,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -559,9 +559,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2523AFC6-E9D3-42BA-B8E2-DF666CE4C56C}">
   <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -615,7 +613,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -699,7 +697,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -837,11 +835,12 @@
   <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="2" max="2" width="8.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>